<commit_message>
AutoCommit_10 октября 2023 г. 9:25:04_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Инд_1</t>
+  </si>
+  <si>
+    <t>Лаб1</t>
+  </si>
+  <si>
+    <t>Баскаков сергей</t>
   </si>
 </sst>
 </file>
@@ -171,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -184,6 +190,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -488,13 +497,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -533,7 +542,9 @@
       <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -612,7 +623,9 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -824,7 +837,9 @@
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -838,7 +853,9 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -908,7 +925,9 @@
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2">
+        <v>5</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -936,6 +955,14 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="2:3" ht="13" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_10 октября 2023 г. 9:30:37_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -188,11 +188,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -500,10 +500,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -514,29 +514,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -626,7 +626,9 @@
       <c r="C9" s="2">
         <v>5</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -654,7 +656,9 @@
         <v>7</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -668,7 +672,9 @@
         <v>8</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -780,7 +786,9 @@
         <v>16</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -794,7 +802,9 @@
         <v>17</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2">
+        <v>5</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -808,7 +818,9 @@
         <v>18</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -824,7 +836,9 @@
       <c r="C23" s="2">
         <v>5</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -957,7 +971,7 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="2:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C33">

</xml_diff>

<commit_message>
AutoCommit_10 октября 2023 г. 9:34:26_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -500,10 +500,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,9 @@
       <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -642,7 +644,9 @@
         <v>6</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -702,7 +706,9 @@
         <v>10</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -854,7 +860,9 @@
       <c r="C24" s="2">
         <v>5</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -898,7 +906,9 @@
         <v>23</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>5</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -956,7 +966,9 @@
         <v>27</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>5</v>
+      </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_23 октября 2023 г. 10:39:12_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -105,13 +105,19 @@
     <t>Чередова Елизавета</t>
   </si>
   <si>
-    <t>Инд_1</t>
-  </si>
-  <si>
     <t>Лаб1</t>
   </si>
   <si>
     <t>Баскаков сергей</t>
+  </si>
+  <si>
+    <t>Инд2</t>
+  </si>
+  <si>
+    <t>Инд1</t>
+  </si>
+  <si>
+    <t>Лаб2</t>
   </si>
 </sst>
 </file>
@@ -503,7 +509,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -540,13 +546,17 @@
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -598,7 +608,9 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
@@ -984,7 +996,7 @@
     </row>
     <row r="33" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_23 октября 2023 г. 10:42:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -506,10 +506,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -948,7 +948,9 @@
         <v>25</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_23 октября 2023 г. 10:44:43_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -506,10 +506,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,9 @@
         <v>3</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -790,8 +792,12 @@
         <v>15</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 16:04:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -509,7 +509,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -544,31 +544,30 @@
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
     </row>
-    <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -578,15 +577,14 @@
       <c r="C5" s="2">
         <v>3</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>5</v>
-      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -597,10 +595,9 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -609,14 +606,13 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2"/>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -627,10 +623,9 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -643,14 +638,13 @@
       <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -658,15 +652,14 @@
         <v>6</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -674,15 +667,14 @@
         <v>7</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -690,15 +682,14 @@
         <v>8</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -709,10 +700,9 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -720,15 +710,14 @@
         <v>10</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2">
-        <v>5</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -739,10 +728,9 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -753,10 +741,9 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -767,10 +754,9 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -781,10 +767,9 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -795,14 +780,13 @@
       <c r="D19" s="2">
         <v>5</v>
       </c>
-      <c r="E19" s="2">
-        <v>5</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -810,15 +794,14 @@
         <v>16</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -826,15 +809,14 @@
         <v>17</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -842,15 +824,14 @@
         <v>18</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -860,15 +841,14 @@
       <c r="C23" s="2">
         <v>5</v>
       </c>
-      <c r="D23" s="2">
-        <v>5</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -878,15 +858,14 @@
       <c r="C24" s="2">
         <v>5</v>
       </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="F24" s="2">
+        <v>5</v>
+      </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -899,10 +878,9 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -913,10 +891,9 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -924,15 +901,14 @@
         <v>23</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2">
-        <v>5</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -943,10 +919,9 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -954,15 +929,14 @@
         <v>25</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="2">
-        <v>5</v>
-      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -975,10 +949,9 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -986,20 +959,18 @@
         <v>27</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="2">
-        <v>5</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="F31" s="2">
+        <v>5</v>
+      </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="2:3" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 16:06:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -506,10 +506,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:W1"/>
+      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -915,7 +915,9 @@
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2">
+        <v>5</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 16:08:00_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Лаб2</t>
+  </si>
+  <si>
+    <t>Лаб3</t>
+  </si>
+  <si>
+    <t>Лаб4</t>
   </si>
 </sst>
 </file>
@@ -506,10 +512,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -553,18 +559,22 @@
         <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -580,8 +590,7 @@
       <c r="D5" s="2">
         <v>5</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -593,8 +602,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -606,11 +614,10 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -621,8 +628,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -638,8 +644,7 @@
       <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>5</v>
       </c>
       <c r="H9" s="2"/>
@@ -653,8 +658,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>5</v>
       </c>
       <c r="H10" s="2"/>
@@ -667,9 +671,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2">
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
         <v>5</v>
       </c>
       <c r="H11" s="2"/>
@@ -683,8 +688,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>5</v>
       </c>
       <c r="H12" s="2"/>
@@ -698,8 +702,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -711,8 +714,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>5</v>
       </c>
       <c r="H14" s="2"/>
@@ -726,8 +728,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -739,8 +740,7 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -752,8 +752,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -764,9 +763,10 @@
         <v>14</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="2">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -780,8 +780,7 @@
       <c r="D19" s="2">
         <v>5</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>5</v>
       </c>
       <c r="H19" s="2"/>
@@ -795,8 +794,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>5</v>
       </c>
       <c r="H20" s="2"/>
@@ -810,8 +808,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>5</v>
       </c>
       <c r="H21" s="2"/>
@@ -825,8 +822,7 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>5</v>
       </c>
       <c r="H22" s="2"/>
@@ -842,8 +838,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>5</v>
       </c>
       <c r="H23" s="2"/>
@@ -859,8 +854,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>5</v>
       </c>
       <c r="H24" s="2"/>
@@ -876,8 +870,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -889,8 +882,7 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -902,8 +894,7 @@
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>5</v>
       </c>
       <c r="H27" s="2"/>
@@ -918,9 +909,10 @@
       <c r="C28" s="2">
         <v>5</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -932,8 +924,7 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>5</v>
       </c>
       <c r="H29" s="2"/>
@@ -949,8 +940,7 @@
         <v>5</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -962,8 +952,7 @@
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>5</v>
       </c>
       <c r="H31" s="2"/>
@@ -971,8 +960,7 @@
     <row r="32" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="2:3" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 16:09:02_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -120,10 +120,10 @@
     <t>Лаб2</t>
   </si>
   <si>
-    <t>Лаб3</t>
-  </si>
-  <si>
-    <t>Лаб4</t>
+    <t>Инд3</t>
+  </si>
+  <si>
+    <t>Инд4</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:W1"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -766,6 +766,12 @@
       <c r="D18" s="2">
         <v>5</v>
       </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 16:11:40_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -512,10 +512,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -674,6 +674,9 @@
       <c r="D11" s="2">
         <v>5</v>
       </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
       <c r="G11" s="2">
         <v>5</v>
       </c>
@@ -786,6 +789,9 @@
       <c r="D19" s="2">
         <v>5</v>
       </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
       <c r="G19" s="2">
         <v>5</v>
       </c>
@@ -844,6 +850,9 @@
         <v>5</v>
       </c>
       <c r="D23" s="2"/>
+      <c r="E23">
+        <v>5</v>
+      </c>
       <c r="G23" s="2">
         <v>5</v>
       </c>
@@ -916,6 +925,9 @@
         <v>5</v>
       </c>
       <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28">
         <v>5</v>
       </c>
       <c r="G28" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 16:16:52_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Инд4</t>
+  </si>
+  <si>
+    <t>Лаб5</t>
   </si>
 </sst>
 </file>
@@ -189,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -201,6 +204,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -512,10 +518,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -526,29 +532,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -569,6 +575,9 @@
       </c>
       <c r="H3" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -677,6 +686,9 @@
       <c r="E11">
         <v>5</v>
       </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
       <c r="G11" s="2">
         <v>5</v>
       </c>
@@ -746,7 +758,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -758,7 +770,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -778,7 +790,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -792,12 +804,20 @@
       <c r="E19">
         <v>5</v>
       </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
       <c r="G19" s="2">
         <v>5</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="2">
+        <v>5</v>
+      </c>
+      <c r="I19" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -811,7 +831,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -825,7 +845,7 @@
       </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -839,7 +859,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -853,12 +873,15 @@
       <c r="E23">
         <v>5</v>
       </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
       <c r="G23" s="2">
         <v>5</v>
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -874,7 +897,7 @@
       </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -888,7 +911,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -900,7 +923,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -914,7 +937,7 @@
       </c>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -930,10 +953,13 @@
       <c r="E28">
         <v>5</v>
       </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -947,7 +973,7 @@
       </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -958,10 +984,12 @@
         <v>5</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="G30" s="2">
+        <v>5</v>
+      </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -975,7 +1003,7 @@
       </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="G32" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 16:21:54_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -212,8 +212,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -221,6 +219,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -528,10 +528,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I19" activeCellId="2" sqref="H7 H19 I19"/>
+      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -542,29 +542,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -603,10 +603,10 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>3</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>5</v>
       </c>
       <c r="G5" s="2"/>
@@ -633,8 +633,11 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
+      <c r="E7">
+        <v>5</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <v>5</v>
       </c>
     </row>
@@ -657,13 +660,13 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="7">
-        <v>5</v>
-      </c>
-      <c r="D9" s="7">
-        <v>5</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="C9" s="5">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="G9" s="5">
         <v>5</v>
       </c>
       <c r="H9" s="2"/>
@@ -677,7 +680,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>5</v>
       </c>
       <c r="H10" s="2"/>
@@ -690,16 +693,16 @@
         <v>7</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="7">
-        <v>5</v>
-      </c>
-      <c r="E11" s="8">
-        <v>5</v>
-      </c>
-      <c r="F11" s="8">
-        <v>5</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5">
         <v>5</v>
       </c>
       <c r="H11" s="2"/>
@@ -713,7 +716,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <v>5</v>
       </c>
       <c r="H12" s="2"/>
@@ -739,7 +742,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="G14" s="7">
+      <c r="G14" s="5">
         <v>5</v>
       </c>
       <c r="H14" s="2"/>
@@ -788,13 +791,13 @@
         <v>14</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="7">
-        <v>5</v>
-      </c>
-      <c r="E18" s="8">
-        <v>5</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="6">
+        <v>5</v>
+      </c>
+      <c r="F18" s="6">
         <v>5</v>
       </c>
       <c r="G18" s="2"/>
@@ -808,22 +811,22 @@
         <v>15</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="7">
-        <v>5</v>
-      </c>
-      <c r="E19" s="8">
-        <v>5</v>
-      </c>
-      <c r="F19" s="8">
-        <v>5</v>
-      </c>
-      <c r="G19" s="7">
-        <v>5</v>
-      </c>
-      <c r="H19" s="7">
-        <v>5</v>
-      </c>
-      <c r="I19" s="9">
+      <c r="D19" s="5">
+        <v>5</v>
+      </c>
+      <c r="E19" s="6">
+        <v>5</v>
+      </c>
+      <c r="F19" s="6">
+        <v>5</v>
+      </c>
+      <c r="G19" s="5">
+        <v>5</v>
+      </c>
+      <c r="H19" s="5">
+        <v>5</v>
+      </c>
+      <c r="I19" s="7">
         <v>5</v>
       </c>
     </row>
@@ -836,7 +839,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="G20" s="7">
+      <c r="G20" s="5">
         <v>5</v>
       </c>
       <c r="H20" s="2"/>
@@ -849,8 +852,13 @@
         <v>17</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="G21" s="7">
+      <c r="D21" s="2">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5">
         <v>5</v>
       </c>
       <c r="H21" s="2"/>
@@ -864,7 +872,10 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="G22" s="7">
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="G22" s="5">
         <v>5</v>
       </c>
       <c r="H22" s="2"/>
@@ -876,17 +887,17 @@
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>5</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="8">
-        <v>5</v>
-      </c>
-      <c r="F23" s="8">
-        <v>5</v>
-      </c>
-      <c r="G23" s="7">
+      <c r="E23" s="6">
+        <v>5</v>
+      </c>
+      <c r="F23" s="6">
+        <v>5</v>
+      </c>
+      <c r="G23" s="5">
         <v>5</v>
       </c>
       <c r="H23" s="2"/>
@@ -898,11 +909,11 @@
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="5">
         <v>5</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="G24" s="7">
+      <c r="G24" s="5">
         <v>5</v>
       </c>
       <c r="H24" s="2"/>
@@ -914,7 +925,7 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="5">
         <v>5</v>
       </c>
       <c r="D25" s="2"/>
@@ -929,7 +940,12 @@
         <v>22</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
@@ -940,12 +956,27 @@
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="G27" s="7">
-        <v>5</v>
-      </c>
-      <c r="H27" s="2"/>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27" s="5">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -954,16 +985,16 @@
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="7">
-        <v>5</v>
-      </c>
-      <c r="D28" s="7">
-        <v>5</v>
-      </c>
-      <c r="E28" s="8">
-        <v>5</v>
-      </c>
-      <c r="F28" s="8">
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
+      <c r="D28" s="5">
+        <v>5</v>
+      </c>
+      <c r="E28" s="6">
+        <v>5</v>
+      </c>
+      <c r="F28" s="6">
         <v>5</v>
       </c>
       <c r="G28" s="2"/>
@@ -978,10 +1009,21 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="G29" s="7">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2"/>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29" s="5">
+        <v>5</v>
+      </c>
+      <c r="H29" s="2">
+        <v>5</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -990,11 +1032,11 @@
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="5">
         <v>5</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="G30" s="7">
+      <c r="G30" s="5">
         <v>5</v>
       </c>
       <c r="H30" s="2"/>
@@ -1008,7 +1050,7 @@
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="G31" s="7">
+      <c r="G31" s="5">
         <v>5</v>
       </c>
       <c r="H31" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_14 ноября 2023 г. 14:46:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -529,10 +529,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -714,7 +714,9 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="G10" s="5">
         <v>5</v>
@@ -722,7 +724,7 @@
       <c r="H10" s="2"/>
       <c r="K10" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M10">
         <v>3</v>
@@ -804,7 +806,9 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="G14" s="5">
         <v>5</v>
@@ -812,7 +816,7 @@
       <c r="H14" s="2"/>
       <c r="K14" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M14">
         <v>3</v>
@@ -1231,7 +1235,9 @@
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2">
+        <v>5</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="G31" s="5">
         <v>5</v>
@@ -1239,7 +1245,7 @@
       <c r="H31" s="2"/>
       <c r="K31" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M31">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_16 ноября 2023 г. 9:22:48_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Лаб5</t>
+  </si>
+  <si>
+    <t>ё</t>
   </si>
 </sst>
 </file>
@@ -529,10 +532,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -767,14 +770,22 @@
         <v>8</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
       <c r="G12" s="5">
         <v>5</v>
       </c>
       <c r="H12" s="2"/>
       <c r="K12" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="M12">
         <v>3</v>
@@ -809,14 +820,19 @@
       <c r="C14" s="2">
         <v>5</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
       <c r="G14" s="5">
         <v>5</v>
       </c>
       <c r="H14" s="2"/>
       <c r="K14" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M14">
         <v>3</v>
@@ -831,6 +847,9 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="K15" s="8">
@@ -1238,14 +1257,19 @@
       <c r="C31" s="2">
         <v>5</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
       <c r="G31" s="5">
         <v>5</v>
       </c>
       <c r="H31" s="2"/>
       <c r="K31" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M31">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_16 ноября 2023 г. 9:24:56_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Лаб5</t>
-  </si>
-  <si>
-    <t>ё</t>
   </si>
 </sst>
 </file>
@@ -532,10 +529,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -826,13 +823,16 @@
       <c r="E14">
         <v>5</v>
       </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
       <c r="G14" s="5">
         <v>5</v>
       </c>
       <c r="H14" s="2"/>
       <c r="K14" s="8">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M14">
         <v>3</v>
@@ -847,14 +847,17 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" t="s">
-        <v>36</v>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="K15" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M15">
         <v>2</v>
@@ -1263,13 +1266,16 @@
       <c r="E31">
         <v>5</v>
       </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
       <c r="G31" s="5">
         <v>5</v>
       </c>
       <c r="H31" s="2"/>
       <c r="K31" s="8">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M31">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_16 ноября 2023 г. 9:28:34_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -529,10 +529,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -610,11 +610,15 @@
       <c r="D5" s="5">
         <v>5</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
       <c r="K5">
         <f>SUM(C5:I5)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M5">
         <v>3</v>
@@ -853,11 +857,13 @@
       <c r="F15">
         <v>5</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="K15" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M15">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_19 ноября 2023 г. 15:16:40_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -529,10 +529,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>5</v>
       </c>
       <c r="D10" s="2"/>
@@ -771,7 +771,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2">
+      <c r="D12" s="5">
         <v>5</v>
       </c>
       <c r="E12">
@@ -818,10 +818,10 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
         <v>5</v>
       </c>
       <c r="E14">
@@ -997,7 +997,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2">
+      <c r="D21" s="5">
         <v>5</v>
       </c>
       <c r="E21">
@@ -1120,7 +1120,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2">
+      <c r="D26" s="5">
         <v>5</v>
       </c>
       <c r="E26">
@@ -1143,10 +1143,10 @@
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
+      <c r="D27" s="5">
         <v>5</v>
       </c>
       <c r="E27">
@@ -1263,10 +1263,10 @@
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="2">
-        <v>5</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="C31" s="5">
+        <v>5</v>
+      </c>
+      <c r="D31" s="5">
         <v>5</v>
       </c>
       <c r="E31">

</xml_diff>

<commit_message>
AutoCommit_21 ноября 2023 г. 10:19:43_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -529,10 +529,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -857,7 +857,7 @@
       <c r="F15" s="6">
         <v>5</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="5">
         <v>5</v>
       </c>
       <c r="H15" s="2"/>
@@ -1158,10 +1158,10 @@
       <c r="G27" s="5">
         <v>5</v>
       </c>
-      <c r="H27" s="2">
-        <v>5</v>
-      </c>
-      <c r="I27">
+      <c r="H27" s="5">
+        <v>5</v>
+      </c>
+      <c r="I27" s="6">
         <v>5</v>
       </c>
       <c r="K27" s="8">
@@ -1219,10 +1219,10 @@
       <c r="G29" s="5">
         <v>5</v>
       </c>
-      <c r="H29" s="2">
-        <v>5</v>
-      </c>
-      <c r="I29">
+      <c r="H29" s="5">
+        <v>5</v>
+      </c>
+      <c r="I29" s="6">
         <v>5</v>
       </c>
       <c r="K29" s="8">

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 22:08:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -529,10 +529,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -799,13 +799,15 @@
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="K13" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M13">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 23:13:57_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -529,10 +529,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -721,14 +721,16 @@
       <c r="C10" s="5">
         <v>5</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
       <c r="G10" s="5">
         <v>5</v>
       </c>
       <c r="H10" s="2"/>
       <c r="K10" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M10">
         <v>3</v>
@@ -926,11 +928,13 @@
       <c r="F18" s="6">
         <v>5</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2">
+        <v>5</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="K18" s="8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="M18">
         <v>5</v>
@@ -1193,11 +1197,13 @@
       <c r="F28" s="6">
         <v>5</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2">
+        <v>5</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="K28" s="8">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M28">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 23:18:53_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -529,10 +529,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -611,14 +611,14 @@
         <v>5</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="2">
         <v>5</v>
       </c>
       <c r="K5">
         <f>SUM(C5:I5)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="M5">
         <v>3</v>
@@ -805,11 +805,13 @@
         <v>5</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="K13" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M13">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_4 декабря 2023 г. 12:16:04_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Лаб5</t>
+  </si>
+  <si>
+    <t>Инд5</t>
+  </si>
+  <si>
+    <t>Инд6</t>
+  </si>
+  <si>
+    <t>Инд7</t>
   </si>
 </sst>
 </file>
@@ -157,7 +166,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +176,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +234,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -532,7 +549,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -582,20 +599,29 @@
         <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -604,24 +630,17 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
-        <v>3</v>
+      <c r="C5" s="8">
+        <v>5</v>
       </c>
       <c r="D5" s="5">
         <v>5</v>
       </c>
-      <c r="G5" s="2">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <f>SUM(C5:I5)</f>
-        <v>18</v>
-      </c>
-      <c r="M5">
-        <v>3</v>
+      <c r="J5" s="2">
+        <v>5</v>
+      </c>
+      <c r="K5" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -633,15 +652,8 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="K6" s="8">
-        <f t="shared" ref="K6:K31" si="0">SUM(C6:I6)</f>
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -655,16 +667,9 @@
       <c r="E7" s="6">
         <v>5</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="5">
-        <v>5</v>
-      </c>
-      <c r="K7" s="8">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M7">
-        <v>4</v>
+      <c r="J7" s="2"/>
+      <c r="K7" s="5">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -676,15 +681,8 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="K8" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>2</v>
-      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -699,17 +697,10 @@
       <c r="D9" s="5">
         <v>5</v>
       </c>
-      <c r="G9" s="5">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="K9" s="8">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
+      <c r="J9" s="5">
+        <v>5</v>
+      </c>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -724,17 +715,10 @@
       <c r="D10" s="2">
         <v>5</v>
       </c>
-      <c r="G10" s="5">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="K10" s="8">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
+      <c r="J10" s="5">
+        <v>5</v>
+      </c>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -753,17 +737,10 @@
       <c r="F11" s="6">
         <v>5</v>
       </c>
-      <c r="G11" s="5">
-        <v>5</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="K11" s="8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M11">
-        <v>5</v>
-      </c>
+      <c r="J11" s="5">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -782,17 +759,10 @@
       <c r="F12" s="6">
         <v>5</v>
       </c>
-      <c r="G12" s="5">
-        <v>5</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="K12" s="8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M12">
-        <v>3</v>
-      </c>
+      <c r="J12" s="5">
+        <v>5</v>
+      </c>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -805,17 +775,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="G13" s="2">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="K13" s="8">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M13">
-        <v>2</v>
-      </c>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -836,17 +799,10 @@
       <c r="F14" s="6">
         <v>5</v>
       </c>
-      <c r="G14" s="5">
-        <v>5</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="K14" s="8">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M14">
-        <v>3</v>
-      </c>
+      <c r="J14" s="5">
+        <v>5</v>
+      </c>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -863,17 +819,10 @@
       <c r="F15" s="6">
         <v>5</v>
       </c>
-      <c r="G15" s="5">
-        <v>5</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="K15" s="8">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M15">
-        <v>2</v>
-      </c>
+      <c r="J15" s="5">
+        <v>5</v>
+      </c>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -884,17 +833,10 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="K16" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -903,17 +845,10 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="K17" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -930,19 +865,18 @@
       <c r="F18" s="6">
         <v>5</v>
       </c>
-      <c r="G18" s="2">
-        <v>5</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="K18" s="8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -959,24 +893,23 @@
       <c r="F19" s="6">
         <v>5</v>
       </c>
-      <c r="G19" s="5">
-        <v>5</v>
-      </c>
-      <c r="H19" s="5">
-        <v>5</v>
-      </c>
-      <c r="I19" s="7">
-        <v>5</v>
-      </c>
-      <c r="K19" s="8">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19" s="5">
+        <v>5</v>
+      </c>
+      <c r="K19" s="5">
+        <v>5</v>
+      </c>
+      <c r="L19" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -985,19 +918,12 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="G20" s="5">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="K20" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="M20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="5">
+        <v>5</v>
+      </c>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1011,19 +937,12 @@
       <c r="E21" s="6">
         <v>5</v>
       </c>
-      <c r="G21" s="5">
-        <v>5</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="K21" s="8">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="5">
+        <v>5</v>
+      </c>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1035,19 +954,12 @@
       <c r="E22" s="6">
         <v>5</v>
       </c>
-      <c r="G22" s="5">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="K22" s="8">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="5">
+        <v>5</v>
+      </c>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -1064,19 +976,12 @@
       <c r="F23" s="6">
         <v>5</v>
       </c>
-      <c r="G23" s="5">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="K23" s="8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="5">
+        <v>5</v>
+      </c>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1087,19 +992,12 @@
         <v>5</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="G24" s="5">
-        <v>5</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="K24" s="8">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="5">
+        <v>5</v>
+      </c>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1110,17 +1008,10 @@
         <v>5</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="K25" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="M25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -1134,17 +1025,10 @@
       <c r="E26" s="6">
         <v>4</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="K26" s="8">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="M26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1163,24 +1047,17 @@
       <c r="F27" s="6">
         <v>5</v>
       </c>
-      <c r="G27" s="5">
-        <v>5</v>
-      </c>
-      <c r="H27" s="5">
-        <v>5</v>
-      </c>
-      <c r="I27" s="6">
-        <v>5</v>
-      </c>
-      <c r="K27" s="8">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="5">
+        <v>5</v>
+      </c>
+      <c r="K27" s="5">
+        <v>5</v>
+      </c>
+      <c r="L27" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1199,19 +1076,12 @@
       <c r="F28" s="6">
         <v>5</v>
       </c>
-      <c r="G28" s="2">
-        <v>5</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="K28" s="8">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="2">
+        <v>5</v>
+      </c>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1226,24 +1096,17 @@
       <c r="F29" s="6">
         <v>5</v>
       </c>
-      <c r="G29" s="5">
-        <v>5</v>
-      </c>
-      <c r="H29" s="5">
-        <v>5</v>
-      </c>
-      <c r="I29" s="6">
-        <v>5</v>
-      </c>
-      <c r="K29" s="8">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="5">
+        <v>5</v>
+      </c>
+      <c r="K29" s="5">
+        <v>5</v>
+      </c>
+      <c r="L29" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1254,19 +1117,12 @@
         <v>5</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="G30" s="5">
-        <v>5</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="K30" s="8">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="5">
+        <v>5</v>
+      </c>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1285,23 +1141,16 @@
       <c r="F31" s="6">
         <v>5</v>
       </c>
-      <c r="G31" s="5">
-        <v>5</v>
-      </c>
-      <c r="H31" s="2"/>
-      <c r="K31" s="8">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="5">
+        <v>5</v>
+      </c>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
@@ -1316,30 +1165,6 @@
   <mergeCells count="1">
     <mergeCell ref="C1:W1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K5:K31">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M31">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_28 декабря 2023 г. 10:38:39_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -546,7 +546,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6:P6"/>
+      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -659,8 +659,19 @@
         <v>3</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
       <c r="F6" s="6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
         <v>5</v>
       </c>
       <c r="L6" s="2"/>
@@ -723,6 +734,15 @@
       <c r="E9" s="2">
         <v>5</v>
       </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
       <c r="L9" s="5">
         <v>5</v>
       </c>
@@ -779,6 +799,12 @@
         <v>5</v>
       </c>
       <c r="G11" s="6">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
         <v>5</v>
       </c>
       <c r="L11" s="5">
@@ -885,7 +911,9 @@
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -983,6 +1011,9 @@
       <c r="G19" s="9">
         <v>5</v>
       </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
       <c r="I19">
         <v>5</v>
       </c>
@@ -1128,6 +1159,9 @@
       <c r="F25" s="6">
         <v>4</v>
       </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
@@ -1152,6 +1186,9 @@
         <v>5</v>
       </c>
       <c r="G26" s="6">
+        <v>5</v>
+      </c>
+      <c r="H26">
         <v>5</v>
       </c>
       <c r="I26">
@@ -1283,6 +1320,12 @@
         <v>5</v>
       </c>
       <c r="G30" s="6">
+        <v>5</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30">
         <v>5</v>
       </c>
       <c r="L30" s="5">

</xml_diff>

<commit_message>
AutoCommit_28 декабря 2023 г. 10:49:04_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>Инд8</t>
+  </si>
+  <si>
+    <t>Лаб3</t>
+  </si>
+  <si>
+    <t>Лаб4</t>
   </si>
 </sst>
 </file>
@@ -540,13 +546,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -557,12 +563,12 @@
     <col min="4" max="8" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -594,10 +600,16 @@
         <v>32</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>0</f>
         <v>0</v>
@@ -607,7 +619,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <f>IF(B4=C4,A3+1,"-----------------")</f>
         <v>1</v>
@@ -624,14 +636,32 @@
       <c r="E4" s="5">
         <v>5</v>
       </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
       <c r="L4" s="2">
         <v>5</v>
       </c>
       <c r="M4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <f t="shared" ref="A5:A30" si="0">IF(B5=C5,A4+1,"-----------------")</f>
         <v>2</v>
@@ -647,7 +677,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -674,12 +704,18 @@
       <c r="J6">
         <v>5</v>
       </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -695,7 +731,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -717,7 +753,7 @@
       </c>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -748,7 +784,7 @@
       </c>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -780,7 +816,7 @@
       </c>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -812,7 +848,7 @@
       </c>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -832,7 +868,7 @@
       </c>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -858,9 +894,11 @@
       <c r="L13" s="5">
         <v>5</v>
       </c>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -884,7 +922,7 @@
       </c>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -900,7 +938,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -918,7 +956,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -953,7 +991,7 @@
       </c>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -986,11 +1024,11 @@
       <c r="M18" s="5">
         <v>5</v>
       </c>
-      <c r="N18" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P18" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1029,11 +1067,11 @@
       <c r="M19" s="2">
         <v>5</v>
       </c>
-      <c r="N19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1056,7 +1094,7 @@
       </c>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1077,7 +1115,7 @@
       </c>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1098,12 +1136,15 @@
       <c r="G22" s="6">
         <v>5</v>
       </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
       <c r="L22" s="5">
         <v>5</v>
       </c>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1121,9 +1162,11 @@
       <c r="L23" s="5">
         <v>5</v>
       </c>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1141,7 +1184,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1162,10 +1205,12 @@
       <c r="I25">
         <v>5</v>
       </c>
-      <c r="L25" s="2"/>
+      <c r="L25" s="2">
+        <v>5</v>
+      </c>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1206,11 +1251,11 @@
       <c r="M26" s="5">
         <v>5</v>
       </c>
-      <c r="N26" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P26" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1250,7 +1295,7 @@
       </c>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1275,11 +1320,11 @@
       <c r="M28" s="5">
         <v>5</v>
       </c>
-      <c r="N28" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P28" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1299,7 +1344,7 @@
       </c>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1328,18 +1373,21 @@
       <c r="J30">
         <v>5</v>
       </c>
+      <c r="K30">
+        <v>5</v>
+      </c>
       <c r="L30" s="5">
         <v>5</v>
       </c>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:14" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.25">
       <c r="C32" s="4" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_28 декабря 2023 г. 10:55:30_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -552,7 +552,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
+      <selection pane="bottomRight" activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1110,10 +1110,19 @@
       <c r="F21" s="6">
         <v>5</v>
       </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
       <c r="L21" s="5">
         <v>5</v>
       </c>
       <c r="M21" s="2"/>
+      <c r="P21">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10">

</xml_diff>

<commit_message>
AutoCommit_28 декабря 2023 г. 14:46:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>2ОИБАС1322: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Лаб1</t>
   </si>
   <si>
-    <t>Баскаков сергей</t>
-  </si>
-  <si>
     <t>Инд2</t>
   </si>
   <si>
@@ -145,13 +142,16 @@
   </si>
   <si>
     <t>Лаб4</t>
+  </si>
+  <si>
+    <t>Сумма</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -163,13 +163,8 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,12 +174,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -216,18 +205,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -237,11 +220,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -546,13 +526,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomRight" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -563,53 +543,53 @@
     <col min="4" max="8" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="10" t="s">
+    <row r="1" spans="1:19" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="P2" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>0</f>
         <v>0</v>
@@ -618,9 +598,12 @@
       <c r="E3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="R3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <f>IF(B4=C4,A3+1,"-----------------")</f>
         <v>1</v>
       </c>
@@ -630,39 +613,46 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8">
-        <v>5</v>
-      </c>
-      <c r="E4" s="5">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="L4" s="2">
-        <v>5</v>
-      </c>
-      <c r="M4" s="2">
-        <v>5</v>
-      </c>
-      <c r="N4">
-        <v>5</v>
-      </c>
-      <c r="O4">
-        <v>5</v>
-      </c>
-      <c r="P4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4">
+        <v>5</v>
+      </c>
+      <c r="L4" s="3">
+        <v>5</v>
+      </c>
+      <c r="M4" s="3">
+        <v>5</v>
+      </c>
+      <c r="N4" s="4">
+        <v>5</v>
+      </c>
+      <c r="O4" s="4">
+        <v>5</v>
+      </c>
+      <c r="P4" s="4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <f>SUM(D4:P4)</f>
+        <v>50</v>
+      </c>
+      <c r="S4" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <f t="shared" ref="A5:A30" si="0">IF(B5=C5,A4+1,"-----------------")</f>
         <v>2</v>
       </c>
@@ -676,9 +666,16 @@
       <c r="E5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="R5" s="6">
+        <f t="shared" ref="R5:R30" si="1">SUM(D5:P5)</f>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -689,34 +686,41 @@
         <v>3</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
-      </c>
-      <c r="K6">
+      <c r="E6" s="3">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5</v>
+      </c>
+      <c r="J6" s="4">
+        <v>5</v>
+      </c>
+      <c r="K6" s="4">
         <v>5</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="5">
-        <v>5</v>
-      </c>
-      <c r="P6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="M6" s="3">
+        <v>5</v>
+      </c>
+      <c r="P6" s="4">
+        <v>5</v>
+      </c>
+      <c r="R6" s="6">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -730,9 +734,16 @@
       <c r="E7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="R7" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -742,19 +753,26 @@
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5">
-        <v>5</v>
-      </c>
-      <c r="E8" s="5">
-        <v>5</v>
-      </c>
-      <c r="L8" s="5">
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+      <c r="L8" s="3">
         <v>5</v>
       </c>
       <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="R8" s="6">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -764,28 +782,35 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="I9">
-        <v>5</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="L9" s="5">
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
+      <c r="G9" s="4">
+        <v>5</v>
+      </c>
+      <c r="I9" s="4">
+        <v>5</v>
+      </c>
+      <c r="J9" s="4">
+        <v>5</v>
+      </c>
+      <c r="L9" s="3">
         <v>5</v>
       </c>
       <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="R9" s="6">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="S9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -796,28 +821,35 @@
         <v>7</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="5">
-        <v>5</v>
-      </c>
-      <c r="F10" s="6">
-        <v>5</v>
-      </c>
-      <c r="G10" s="6">
-        <v>5</v>
-      </c>
-      <c r="I10">
-        <v>5</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="E10" s="3">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>5</v>
+      </c>
+      <c r="G10" s="4">
+        <v>5</v>
+      </c>
+      <c r="I10" s="4">
+        <v>5</v>
+      </c>
+      <c r="J10" s="4">
+        <v>5</v>
+      </c>
+      <c r="L10" s="3">
         <v>5</v>
       </c>
       <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="R10" s="6">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -828,28 +860,35 @@
         <v>8</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="5">
-        <v>5</v>
-      </c>
-      <c r="F11" s="6">
-        <v>5</v>
-      </c>
-      <c r="G11" s="6">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>5</v>
-      </c>
-      <c r="J11">
-        <v>5</v>
-      </c>
-      <c r="L11" s="5">
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5</v>
+      </c>
+      <c r="G11" s="4">
+        <v>5</v>
+      </c>
+      <c r="I11" s="4">
+        <v>5</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5</v>
+      </c>
+      <c r="L11" s="3">
         <v>5</v>
       </c>
       <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="R11" s="6">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="S11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -859,17 +898,24 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>5</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="L12" s="2">
+      <c r="L12" s="3">
         <v>5</v>
       </c>
       <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="R12" s="6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="S12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -879,27 +925,34 @@
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="5">
-        <v>5</v>
-      </c>
-      <c r="E13" s="5">
-        <v>5</v>
-      </c>
-      <c r="F13" s="6">
-        <v>5</v>
-      </c>
-      <c r="G13" s="6">
-        <v>5</v>
-      </c>
-      <c r="L13" s="5">
-        <v>5</v>
-      </c>
-      <c r="M13" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+      <c r="D13" s="3">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4">
+        <v>5</v>
+      </c>
+      <c r="G13" s="4">
+        <v>5</v>
+      </c>
+      <c r="L13" s="3">
+        <v>5</v>
+      </c>
+      <c r="M13" s="3">
+        <v>5</v>
+      </c>
+      <c r="R13" s="6">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="S13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -911,19 +964,26 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="6">
-        <v>5</v>
-      </c>
-      <c r="G14" s="6">
-        <v>5</v>
-      </c>
-      <c r="L14" s="5">
+      <c r="F14" s="4">
+        <v>5</v>
+      </c>
+      <c r="G14" s="4">
+        <v>5</v>
+      </c>
+      <c r="L14" s="3">
         <v>5</v>
       </c>
       <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="R14" s="6">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="S14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -937,9 +997,16 @@
       <c r="E15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="R15" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -949,15 +1016,22 @@
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <v>5</v>
       </c>
       <c r="E16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="R16" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="S16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -968,31 +1042,38 @@
         <v>14</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="5">
-        <v>5</v>
-      </c>
-      <c r="F17" s="6">
-        <v>5</v>
-      </c>
-      <c r="G17" s="6">
-        <v>5</v>
-      </c>
-      <c r="I17">
-        <v>5</v>
-      </c>
-      <c r="J17">
-        <v>5</v>
-      </c>
-      <c r="K17">
-        <v>5</v>
-      </c>
-      <c r="L17" s="2">
+      <c r="E17" s="3">
+        <v>5</v>
+      </c>
+      <c r="F17" s="4">
+        <v>5</v>
+      </c>
+      <c r="G17" s="4">
+        <v>5</v>
+      </c>
+      <c r="I17" s="4">
+        <v>5</v>
+      </c>
+      <c r="J17" s="4">
+        <v>5</v>
+      </c>
+      <c r="K17" s="4">
+        <v>5</v>
+      </c>
+      <c r="L17" s="3">
         <v>5</v>
       </c>
       <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+      <c r="R17" s="6">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="S17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1003,33 +1084,40 @@
         <v>15</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="5">
-        <v>5</v>
-      </c>
-      <c r="F18" s="6">
-        <v>5</v>
-      </c>
-      <c r="G18" s="6">
-        <v>5</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
-      </c>
-      <c r="J18">
-        <v>5</v>
-      </c>
-      <c r="L18" s="5">
-        <v>5</v>
-      </c>
-      <c r="M18" s="5">
-        <v>5</v>
-      </c>
-      <c r="P18" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="E18" s="3">
+        <v>5</v>
+      </c>
+      <c r="F18" s="4">
+        <v>5</v>
+      </c>
+      <c r="G18" s="4">
+        <v>5</v>
+      </c>
+      <c r="I18" s="4">
+        <v>5</v>
+      </c>
+      <c r="J18" s="4">
+        <v>5</v>
+      </c>
+      <c r="L18" s="3">
+        <v>5</v>
+      </c>
+      <c r="M18" s="3">
+        <v>5</v>
+      </c>
+      <c r="P18" s="5">
+        <v>5</v>
+      </c>
+      <c r="R18" s="6">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1040,39 +1128,46 @@
         <v>16</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="2">
-        <v>5</v>
-      </c>
-      <c r="F19" s="9">
-        <v>5</v>
-      </c>
-      <c r="G19" s="9">
-        <v>5</v>
-      </c>
-      <c r="H19">
-        <v>5</v>
-      </c>
-      <c r="I19">
-        <v>5</v>
-      </c>
-      <c r="J19">
-        <v>5</v>
-      </c>
-      <c r="K19">
-        <v>5</v>
-      </c>
-      <c r="L19" s="5">
-        <v>5</v>
-      </c>
-      <c r="M19" s="2">
-        <v>5</v>
-      </c>
-      <c r="P19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="E19" s="3">
+        <v>5</v>
+      </c>
+      <c r="F19" s="4">
+        <v>5</v>
+      </c>
+      <c r="G19" s="4">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4">
+        <v>5</v>
+      </c>
+      <c r="I19" s="4">
+        <v>5</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5</v>
+      </c>
+      <c r="K19" s="4">
+        <v>5</v>
+      </c>
+      <c r="L19" s="3">
+        <v>5</v>
+      </c>
+      <c r="M19" s="3">
+        <v>5</v>
+      </c>
+      <c r="P19" s="4">
+        <v>5</v>
+      </c>
+      <c r="R19" s="6">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="S19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1083,19 +1178,26 @@
         <v>17</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="5">
-        <v>5</v>
-      </c>
-      <c r="F20" s="6">
-        <v>5</v>
-      </c>
-      <c r="L20" s="5">
+      <c r="E20" s="3">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4">
+        <v>5</v>
+      </c>
+      <c r="L20" s="3">
         <v>5</v>
       </c>
       <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="R20" s="6">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="S20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1107,25 +1209,32 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="6">
-        <v>5</v>
-      </c>
-      <c r="J21">
-        <v>5</v>
-      </c>
-      <c r="K21">
-        <v>5</v>
-      </c>
-      <c r="L21" s="5">
+      <c r="F21" s="4">
+        <v>5</v>
+      </c>
+      <c r="J21" s="4">
+        <v>5</v>
+      </c>
+      <c r="K21" s="4">
+        <v>5</v>
+      </c>
+      <c r="L21" s="3">
         <v>5</v>
       </c>
       <c r="M21" s="2"/>
-      <c r="P21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="P21" s="4">
+        <v>5</v>
+      </c>
+      <c r="R21" s="6">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="S21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -1135,26 +1244,33 @@
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="3">
         <v>5</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="6">
-        <v>5</v>
-      </c>
-      <c r="G22" s="6">
-        <v>5</v>
-      </c>
-      <c r="K22">
-        <v>5</v>
-      </c>
-      <c r="L22" s="5">
+      <c r="F22" s="4">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4">
+        <v>5</v>
+      </c>
+      <c r="K22" s="4">
+        <v>5</v>
+      </c>
+      <c r="L22" s="3">
         <v>5</v>
       </c>
       <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+      <c r="R22" s="6">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="S22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1164,19 +1280,26 @@
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="3">
         <v>5</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="L23" s="5">
-        <v>5</v>
-      </c>
-      <c r="M23" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="L23" s="3">
+        <v>5</v>
+      </c>
+      <c r="M23" s="3">
+        <v>5</v>
+      </c>
+      <c r="R23" s="6">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="S23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -1186,15 +1309,22 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="3">
         <v>5</v>
       </c>
       <c r="E24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="R24" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="S24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -1205,22 +1335,29 @@
         <v>22</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="5">
-        <v>5</v>
-      </c>
-      <c r="F25" s="6">
+      <c r="E25" s="3">
+        <v>5</v>
+      </c>
+      <c r="F25" s="4">
         <v>4</v>
       </c>
-      <c r="I25">
-        <v>5</v>
-      </c>
-      <c r="L25" s="2">
+      <c r="I25" s="4">
+        <v>5</v>
+      </c>
+      <c r="L25" s="3">
         <v>5</v>
       </c>
       <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+      <c r="R25" s="6">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="S25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -1230,42 +1367,49 @@
       <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="5">
-        <v>5</v>
-      </c>
-      <c r="E26" s="5">
-        <v>5</v>
-      </c>
-      <c r="F26" s="6">
-        <v>5</v>
-      </c>
-      <c r="G26" s="6">
-        <v>5</v>
-      </c>
-      <c r="H26">
-        <v>5</v>
-      </c>
-      <c r="I26">
-        <v>5</v>
-      </c>
-      <c r="J26">
-        <v>5</v>
-      </c>
-      <c r="K26">
-        <v>5</v>
-      </c>
-      <c r="L26" s="5">
-        <v>5</v>
-      </c>
-      <c r="M26" s="5">
-        <v>5</v>
-      </c>
-      <c r="P26" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10">
+      <c r="D26" s="3">
+        <v>5</v>
+      </c>
+      <c r="E26" s="3">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4">
+        <v>5</v>
+      </c>
+      <c r="G26" s="4">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4">
+        <v>5</v>
+      </c>
+      <c r="I26" s="4">
+        <v>5</v>
+      </c>
+      <c r="J26" s="4">
+        <v>5</v>
+      </c>
+      <c r="K26" s="4">
+        <v>5</v>
+      </c>
+      <c r="L26" s="3">
+        <v>5</v>
+      </c>
+      <c r="M26" s="3">
+        <v>5</v>
+      </c>
+      <c r="P26" s="4">
+        <v>5</v>
+      </c>
+      <c r="R26" s="6">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="S26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -1275,37 +1419,44 @@
       <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="5">
-        <v>5</v>
-      </c>
-      <c r="E27" s="5">
-        <v>5</v>
-      </c>
-      <c r="F27" s="6">
-        <v>5</v>
-      </c>
-      <c r="G27" s="6">
-        <v>5</v>
-      </c>
-      <c r="H27">
-        <v>5</v>
-      </c>
-      <c r="I27">
-        <v>5</v>
-      </c>
-      <c r="J27">
-        <v>5</v>
-      </c>
-      <c r="K27">
-        <v>5</v>
-      </c>
-      <c r="L27" s="2">
+      <c r="D27" s="3">
+        <v>5</v>
+      </c>
+      <c r="E27" s="3">
+        <v>5</v>
+      </c>
+      <c r="F27" s="4">
+        <v>5</v>
+      </c>
+      <c r="G27" s="4">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4">
+        <v>5</v>
+      </c>
+      <c r="I27" s="4">
+        <v>5</v>
+      </c>
+      <c r="J27" s="4">
+        <v>5</v>
+      </c>
+      <c r="K27" s="4">
+        <v>5</v>
+      </c>
+      <c r="L27" s="3">
         <v>5</v>
       </c>
       <c r="M27" s="2"/>
-    </row>
-    <row r="28" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10">
+      <c r="R27" s="6">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="S27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -1317,24 +1468,31 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="6">
-        <v>5</v>
-      </c>
-      <c r="G28" s="6">
-        <v>5</v>
-      </c>
-      <c r="L28" s="5">
-        <v>5</v>
-      </c>
-      <c r="M28" s="5">
-        <v>5</v>
-      </c>
-      <c r="P28" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10">
+      <c r="F28" s="4">
+        <v>5</v>
+      </c>
+      <c r="G28" s="4">
+        <v>5</v>
+      </c>
+      <c r="L28" s="3">
+        <v>5</v>
+      </c>
+      <c r="M28" s="3">
+        <v>5</v>
+      </c>
+      <c r="P28" s="4">
+        <v>5</v>
+      </c>
+      <c r="R28" s="6">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="S28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
@@ -1344,17 +1502,24 @@
       <c r="C29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="3">
         <v>5</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="L29" s="5">
+      <c r="L29" s="3">
         <v>5</v>
       </c>
       <c r="M29" s="2"/>
-    </row>
-    <row r="30" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10">
+      <c r="R29" s="6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="S29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -1364,48 +1529,258 @@
       <c r="C30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="5">
-        <v>5</v>
-      </c>
-      <c r="E30" s="5">
-        <v>5</v>
-      </c>
-      <c r="F30" s="6">
-        <v>5</v>
-      </c>
-      <c r="G30" s="6">
-        <v>5</v>
-      </c>
-      <c r="I30">
-        <v>5</v>
-      </c>
-      <c r="J30">
-        <v>5</v>
-      </c>
-      <c r="K30">
-        <v>5</v>
-      </c>
-      <c r="L30" s="5">
+      <c r="D30" s="3">
+        <v>5</v>
+      </c>
+      <c r="E30" s="3">
+        <v>5</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5</v>
+      </c>
+      <c r="G30" s="4">
+        <v>5</v>
+      </c>
+      <c r="I30" s="4">
+        <v>5</v>
+      </c>
+      <c r="J30" s="4">
+        <v>5</v>
+      </c>
+      <c r="K30" s="4">
+        <v>5</v>
+      </c>
+      <c r="L30" s="3">
         <v>5</v>
       </c>
       <c r="M30" s="2"/>
-    </row>
-    <row r="31" spans="1:16" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32">
-        <v>5</v>
-      </c>
-    </row>
+      <c r="R30" s="6">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="3">
+        <v>5</v>
+      </c>
+      <c r="E31" s="3">
+        <v>5</v>
+      </c>
+      <c r="F31" s="4">
+        <v>5</v>
+      </c>
+      <c r="G31" s="4">
+        <v>5</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="4">
+        <v>5</v>
+      </c>
+      <c r="J31" s="4">
+        <v>5</v>
+      </c>
+      <c r="K31" s="4">
+        <v>5</v>
+      </c>
+      <c r="L31" s="3">
+        <v>5</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+    </row>
+    <row r="32" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="3">
+        <v>5</v>
+      </c>
+      <c r="E32" s="3">
+        <v>5</v>
+      </c>
+      <c r="F32" s="4">
+        <v>5</v>
+      </c>
+      <c r="G32" s="4">
+        <v>5</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="4">
+        <v>5</v>
+      </c>
+      <c r="J32" s="4">
+        <v>5</v>
+      </c>
+      <c r="K32" s="4">
+        <v>5</v>
+      </c>
+      <c r="L32" s="3">
+        <v>5</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+    </row>
+    <row r="33" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="3">
+        <v>5</v>
+      </c>
+      <c r="E33" s="3">
+        <v>5</v>
+      </c>
+      <c r="F33" s="4">
+        <v>5</v>
+      </c>
+      <c r="G33" s="4">
+        <v>5</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="4">
+        <v>5</v>
+      </c>
+      <c r="J33" s="4">
+        <v>5</v>
+      </c>
+      <c r="K33" s="4">
+        <v>5</v>
+      </c>
+      <c r="L33" s="3">
+        <v>5</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+    </row>
+    <row r="34" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="3">
+        <v>5</v>
+      </c>
+      <c r="E34" s="3">
+        <v>5</v>
+      </c>
+      <c r="F34" s="4">
+        <v>5</v>
+      </c>
+      <c r="G34" s="4">
+        <v>5</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="4">
+        <v>5</v>
+      </c>
+      <c r="J34" s="4">
+        <v>5</v>
+      </c>
+      <c r="K34" s="4">
+        <v>5</v>
+      </c>
+      <c r="L34" s="3">
+        <v>5</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+    </row>
+    <row r="35" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="3">
+        <v>5</v>
+      </c>
+      <c r="E35" s="3">
+        <v>5</v>
+      </c>
+      <c r="F35" s="4">
+        <v>5</v>
+      </c>
+      <c r="G35" s="4">
+        <v>5</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="4">
+        <v>5</v>
+      </c>
+      <c r="J35" s="4">
+        <v>5</v>
+      </c>
+      <c r="K35" s="4">
+        <v>5</v>
+      </c>
+      <c r="L35" s="3">
+        <v>5</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+    </row>
+    <row r="36" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="3">
+        <v>5</v>
+      </c>
+      <c r="E36" s="3">
+        <v>5</v>
+      </c>
+      <c r="F36" s="4">
+        <v>5</v>
+      </c>
+      <c r="G36" s="4">
+        <v>5</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="4">
+        <v>5</v>
+      </c>
+      <c r="J36" s="4">
+        <v>5</v>
+      </c>
+      <c r="K36" s="4">
+        <v>5</v>
+      </c>
+      <c r="L36" s="3">
+        <v>5</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+    </row>
+    <row r="37" spans="3:16" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <conditionalFormatting sqref="R4:R30">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_30 декабря 2023 г. 23:57:30_SibNout2021
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\2ОИБАС1322_ОпСис_\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Sibirev I. V." sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -164,7 +159,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +169,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -222,6 +223,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -532,23 +535,23 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="8" width="5.1796875" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="8" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="29.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
@@ -589,7 +592,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>0</f>
         <v>0</v>
@@ -602,7 +605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f>IF(B4=C4,A3+1,"-----------------")</f>
         <v>1</v>
@@ -628,6 +631,9 @@
       <c r="I4" s="4">
         <v>5</v>
       </c>
+      <c r="J4" s="9">
+        <v>5</v>
+      </c>
       <c r="L4" s="3">
         <v>5</v>
       </c>
@@ -645,13 +651,13 @@
       </c>
       <c r="R4">
         <f>SUM(D4:P4)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="S4" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" ref="A5:A30" si="0">IF(B5=C5,A4+1,"-----------------")</f>
         <v>2</v>
@@ -674,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -719,7 +725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -742,7 +748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -771,7 +777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -809,7 +815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -848,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -887,7 +893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -914,7 +920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -951,7 +957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -970,19 +976,25 @@
       <c r="G14" s="4">
         <v>5</v>
       </c>
+      <c r="I14" s="8">
+        <v>5</v>
+      </c>
+      <c r="J14" s="8">
+        <v>5</v>
+      </c>
       <c r="L14" s="3">
         <v>5</v>
       </c>
       <c r="M14" s="2"/>
       <c r="R14" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="S14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1005,7 +1017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1030,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1072,7 +1084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1116,7 +1128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1166,7 +1178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1196,7 +1208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1233,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1269,7 +1281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1298,7 +1310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1323,7 +1335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1344,19 +1356,22 @@
       <c r="I25" s="4">
         <v>5</v>
       </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
       <c r="L25" s="3">
         <v>5</v>
       </c>
       <c r="M25" s="2"/>
       <c r="R25" s="6">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="S25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1408,7 +1423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1455,7 +1470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1491,7 +1506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1518,7 +1533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1562,7 +1577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1596,7 +1611,7 @@
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1630,7 +1645,7 @@
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
     </row>
-    <row r="33" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:16" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>27</v>
       </c>
@@ -1664,7 +1679,7 @@
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
     </row>
-    <row r="34" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:16" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>27</v>
       </c>
@@ -1698,7 +1713,7 @@
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
     </row>
-    <row r="35" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:16" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>27</v>
       </c>
@@ -1732,7 +1747,7 @@
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
     </row>
-    <row r="36" spans="3:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:16" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>27</v>
       </c>
@@ -1766,7 +1781,7 @@
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="3:16" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="3:16" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="R4:R30">

</xml_diff>

<commit_message>
AutoCommit_7 января 2024 г. 16:37:12_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
+++ b/2ОИБАС1322_ОпСис_/2ОИБАС1322_ОпСис_.xlsx
@@ -164,7 +164,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -222,6 +228,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -532,7 +540,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -628,6 +636,9 @@
       <c r="I4" s="4">
         <v>5</v>
       </c>
+      <c r="J4" s="9">
+        <v>5</v>
+      </c>
       <c r="L4" s="3">
         <v>5</v>
       </c>
@@ -645,7 +656,7 @@
       </c>
       <c r="R4">
         <f>SUM(D4:P4)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="S4" s="7">
         <v>5</v>
@@ -970,13 +981,19 @@
       <c r="G14" s="4">
         <v>5</v>
       </c>
+      <c r="I14" s="8">
+        <v>5</v>
+      </c>
+      <c r="J14" s="8">
+        <v>5</v>
+      </c>
       <c r="L14" s="3">
         <v>5</v>
       </c>
       <c r="M14" s="2"/>
       <c r="R14" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="S14">
         <v>3</v>
@@ -1208,10 +1225,18 @@
         <v>18</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
       <c r="F21" s="4">
         <v>5</v>
       </c>
+      <c r="G21" s="8">
+        <v>5</v>
+      </c>
+      <c r="I21" s="8">
+        <v>5</v>
+      </c>
       <c r="J21" s="4">
         <v>5</v>
       </c>
@@ -1221,13 +1246,15 @@
       <c r="L21" s="3">
         <v>5</v>
       </c>
-      <c r="M21" s="2"/>
+      <c r="M21" s="2">
+        <v>5</v>
+      </c>
       <c r="P21" s="4">
         <v>5</v>
       </c>
       <c r="R21" s="6">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="S21">
         <v>4</v>
@@ -1344,13 +1371,16 @@
       <c r="I25" s="4">
         <v>5</v>
       </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
       <c r="L25" s="3">
         <v>5</v>
       </c>
       <c r="M25" s="2"/>
       <c r="R25" s="6">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="S25">
         <v>3</v>

</xml_diff>